<commit_message>
Save before adding new server side validation
</commit_message>
<xml_diff>
--- a/journalentry/Content/uploads/JE Spreadsheet.xlsx
+++ b/journalentry/Content/uploads/JE Spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njohnson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njohnson\Documents\Work Docs\Projects\Journal Entry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>88888</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>

</xml_diff>